<commit_message>
A commit to save the current state before I start changing the simulator. The change will be making the TSS be in the middle of the simulation, and not very much to the left...
Signed-off-by: Daniel Gissin <Daniel Gissin>
</commit_message>
<xml_diff>
--- a/clustering/results/wt/Gene_results.xlsx
+++ b/clustering/results/wt/Gene_results.xlsx
@@ -153,31 +153,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -464,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1602,7 +1578,7 @@
   </sheetData>
   <autoFilter ref="A1:D154">
     <sortState ref="A24:D98">
-      <sortCondition sortBy="cellColor" ref="B1:B154" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="B1:B154" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>